<commit_message>
update and fix bug
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C943"/>
+  <dimension ref="A1:C950"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11200,7 +11200,7 @@
         </is>
       </c>
       <c r="C833" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="834">
@@ -11317,7 +11317,7 @@
         </is>
       </c>
       <c r="C842" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="843">
@@ -12058,7 +12058,7 @@
         </is>
       </c>
       <c r="C899" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="900">
@@ -12123,7 +12123,7 @@
         </is>
       </c>
       <c r="C904" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="905">
@@ -12409,7 +12409,7 @@
         </is>
       </c>
       <c r="C926" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="927">
@@ -12418,7 +12418,7 @@
       </c>
       <c r="B927" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="C927" t="n">
@@ -12431,11 +12431,11 @@
       </c>
       <c r="B928" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C928" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="929">
@@ -12444,11 +12444,11 @@
       </c>
       <c r="B929" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C929" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="930">
@@ -12457,24 +12457,24 @@
       </c>
       <c r="B930" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="C930" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="931">
       <c r="A931" s="2" t="n">
-        <v>44148</v>
+        <v>44147</v>
       </c>
       <c r="B931" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>80+</t>
         </is>
       </c>
       <c r="C931" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="932">
@@ -12483,11 +12483,11 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="C932" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="933">
@@ -12496,11 +12496,11 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C933" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="934">
@@ -12509,37 +12509,37 @@
       </c>
       <c r="B934" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C934" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="935">
       <c r="A935" s="2" t="n">
-        <v>44149</v>
+        <v>44148</v>
       </c>
       <c r="B935" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="C935" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="936">
       <c r="A936" s="2" t="n">
-        <v>44149</v>
+        <v>44148</v>
       </c>
       <c r="B936" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>80+</t>
         </is>
       </c>
       <c r="C936" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="937">
@@ -12548,11 +12548,11 @@
       </c>
       <c r="B937" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="C937" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="938">
@@ -12561,11 +12561,11 @@
       </c>
       <c r="B938" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C938" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="939">
@@ -12574,37 +12574,37 @@
       </c>
       <c r="B939" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C939" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="940">
       <c r="A940" s="2" t="n">
-        <v>44150</v>
+        <v>44149</v>
       </c>
       <c r="B940" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="C940" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="941">
       <c r="A941" s="2" t="n">
-        <v>44150</v>
+        <v>44149</v>
       </c>
       <c r="B941" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>80+</t>
         </is>
       </c>
       <c r="C941" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="942">
@@ -12613,11 +12613,11 @@
       </c>
       <c r="B942" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="C942" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="943">
@@ -12626,11 +12626,102 @@
       </c>
       <c r="B943" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C943" t="n">
-        <v>5</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="2" t="n">
+        <v>44150</v>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C944" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="2" t="n">
+        <v>44150</v>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C945" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="2" t="n">
+        <v>44150</v>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C946" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="2" t="n">
+        <v>44151</v>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="C947" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="2" t="n">
+        <v>44151</v>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C948" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="2" t="n">
+        <v>44151</v>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C949" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="2" t="n">
+        <v>44151</v>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C950" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model and datasets
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C973"/>
+  <dimension ref="A1:C983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10277,7 +10277,7 @@
         </is>
       </c>
       <c r="C762" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="763">
@@ -11733,7 +11733,7 @@
         </is>
       </c>
       <c r="C874" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="875">
@@ -12604,7 +12604,7 @@
         </is>
       </c>
       <c r="C941" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="942">
@@ -12682,7 +12682,7 @@
         </is>
       </c>
       <c r="C947" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="948">
@@ -12799,7 +12799,7 @@
         </is>
       </c>
       <c r="C956" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="957">
@@ -12825,7 +12825,7 @@
         </is>
       </c>
       <c r="C958" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="959">
@@ -12851,7 +12851,7 @@
         </is>
       </c>
       <c r="C960" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="961">
@@ -12864,7 +12864,7 @@
         </is>
       </c>
       <c r="C961" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="962">
@@ -12877,7 +12877,7 @@
         </is>
       </c>
       <c r="C962" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="963">
@@ -12903,7 +12903,7 @@
         </is>
       </c>
       <c r="C964" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="965">
@@ -12942,7 +12942,7 @@
         </is>
       </c>
       <c r="C967" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="968">
@@ -12951,11 +12951,11 @@
       </c>
       <c r="B968" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C968" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="969">
@@ -12964,11 +12964,11 @@
       </c>
       <c r="B969" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C969" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="970">
@@ -12977,24 +12977,24 @@
       </c>
       <c r="B970" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="C970" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="971">
       <c r="A971" s="2" t="n">
-        <v>44156</v>
+        <v>44155</v>
       </c>
       <c r="B971" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>80+</t>
         </is>
       </c>
       <c r="C971" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="972">
@@ -13003,11 +13003,11 @@
       </c>
       <c r="B972" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="C972" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="973">
@@ -13016,11 +13016,141 @@
       </c>
       <c r="B973" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C973" t="n">
-        <v>12</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="2" t="n">
+        <v>44156</v>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C974" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="2" t="n">
+        <v>44156</v>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C975" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="2" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="C976" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="2" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="C977" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="2" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C978" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="2" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C979" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="2" t="n">
+        <v>44157</v>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C980" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="2" t="n">
+        <v>44158</v>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C981" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="2" t="n">
+        <v>44158</v>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C982" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="2" t="n">
+        <v>44158</v>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C983" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model and dataset
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C986"/>
+  <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11070,7 +11070,7 @@
         </is>
       </c>
       <c r="C823" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="824">
@@ -11681,7 +11681,7 @@
         </is>
       </c>
       <c r="C870" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="871">
@@ -12734,7 +12734,7 @@
         </is>
       </c>
       <c r="C951" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="952">
@@ -12994,7 +12994,7 @@
         </is>
       </c>
       <c r="C971" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="972">
@@ -13098,7 +13098,7 @@
         </is>
       </c>
       <c r="C979" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="980">
@@ -13111,7 +13111,7 @@
         </is>
       </c>
       <c r="C980" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="981">
@@ -13150,7 +13150,7 @@
         </is>
       </c>
       <c r="C983" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="984">
@@ -13159,11 +13159,11 @@
       </c>
       <c r="B984" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="C984" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="985">
@@ -13172,7 +13172,7 @@
       </c>
       <c r="B985" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="C985" t="n">
@@ -13185,10 +13185,140 @@
       </c>
       <c r="B986" t="inlineStr">
         <is>
-          <t>80+</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="C986" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="2" t="n">
+        <v>44159</v>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C987" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="2" t="n">
+        <v>44160</v>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>40-49</t>
+        </is>
+      </c>
+      <c r="C988" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" s="2" t="n">
+        <v>44160</v>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="C989" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="2" t="n">
+        <v>44160</v>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C990" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="2" t="n">
+        <v>44160</v>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C991" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" s="2" t="n">
+        <v>44160</v>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C992" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="2" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="C993" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="2" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C994" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" s="2" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C995" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="2" t="n">
+        <v>44161</v>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C996" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update datasets & models
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C996"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11213,7 +11213,7 @@
         </is>
       </c>
       <c r="C834" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="835">
@@ -12799,7 +12799,7 @@
         </is>
       </c>
       <c r="C956" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="957">
@@ -12916,7 +12916,7 @@
         </is>
       </c>
       <c r="C965" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="966">
@@ -13046,7 +13046,7 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="976">
@@ -13137,7 +13137,7 @@
         </is>
       </c>
       <c r="C982" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="983">
@@ -13150,7 +13150,7 @@
         </is>
       </c>
       <c r="C983" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="984">
@@ -13176,7 +13176,7 @@
         </is>
       </c>
       <c r="C985" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="986">
@@ -13189,7 +13189,7 @@
         </is>
       </c>
       <c r="C986" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="987">
@@ -13202,7 +13202,7 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="988">
@@ -13241,7 +13241,7 @@
         </is>
       </c>
       <c r="C990" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="991">
@@ -13254,7 +13254,7 @@
         </is>
       </c>
       <c r="C991" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="992">
@@ -13267,7 +13267,7 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="993">
@@ -13280,7 +13280,7 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="994">
@@ -13293,7 +13293,7 @@
         </is>
       </c>
       <c r="C994" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="995">
@@ -13306,7 +13306,7 @@
         </is>
       </c>
       <c r="C995" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="996">
@@ -13319,7 +13319,59 @@
         </is>
       </c>
       <c r="C996" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="2" t="n">
+        <v>44162</v>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="C997" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" s="2" t="n">
+        <v>44162</v>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C998" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="2" t="n">
+        <v>44162</v>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C999" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="2" t="n">
+        <v>44162</v>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C1000" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update datasets and models
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12981,7 +12981,7 @@
         </is>
       </c>
       <c r="C970" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="971">
@@ -13046,7 +13046,7 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="976">
@@ -13319,7 +13319,7 @@
         </is>
       </c>
       <c r="C996" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="997">
@@ -13345,7 +13345,7 @@
         </is>
       </c>
       <c r="C998" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="999">
@@ -13358,7 +13358,7 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="1000">
@@ -13371,7 +13371,46 @@
         </is>
       </c>
       <c r="C1000" t="n">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="2" t="n">
+        <v>44163</v>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>40-49</t>
+        </is>
+      </c>
+      <c r="C1001" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="2" t="n">
+        <v>44163</v>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C1002" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="2" t="n">
+        <v>44163</v>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C1003" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating model and datasets (auto generated commit)
</commit_message>
<xml_diff>
--- a/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
+++ b/data/updated/data_indiana_covid_deaths_by_date_by_age_group.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1016"/>
+  <dimension ref="A1:C1020"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8288,7 +8288,7 @@
         </is>
       </c>
       <c r="C609" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="610">
@@ -12929,7 +12929,7 @@
         </is>
       </c>
       <c r="C966" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="967">
@@ -12942,7 +12942,7 @@
         </is>
       </c>
       <c r="C967" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="968">
@@ -12994,7 +12994,7 @@
         </is>
       </c>
       <c r="C971" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="972">
@@ -13046,7 +13046,7 @@
         </is>
       </c>
       <c r="C975" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="976">
@@ -13098,7 +13098,7 @@
         </is>
       </c>
       <c r="C979" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="980">
@@ -13111,7 +13111,7 @@
         </is>
       </c>
       <c r="C980" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="981">
@@ -13202,7 +13202,7 @@
         </is>
       </c>
       <c r="C987" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="988">
@@ -13241,7 +13241,7 @@
         </is>
       </c>
       <c r="C990" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="991">
@@ -13254,7 +13254,7 @@
         </is>
       </c>
       <c r="C991" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="992">
@@ -13267,7 +13267,7 @@
         </is>
       </c>
       <c r="C992" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="993">
@@ -13280,7 +13280,7 @@
         </is>
       </c>
       <c r="C993" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="994">
@@ -13332,7 +13332,7 @@
         </is>
       </c>
       <c r="C997" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="998">
@@ -13358,7 +13358,7 @@
         </is>
       </c>
       <c r="C999" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1000">
@@ -13371,7 +13371,7 @@
         </is>
       </c>
       <c r="C1000" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1001">
@@ -13384,7 +13384,7 @@
         </is>
       </c>
       <c r="C1001" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1002">
@@ -13436,7 +13436,7 @@
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1006">
@@ -13449,7 +13449,7 @@
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1007">
@@ -13462,7 +13462,7 @@
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="1008">
@@ -13475,7 +13475,7 @@
         </is>
       </c>
       <c r="C1008" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1009">
@@ -13488,7 +13488,7 @@
         </is>
       </c>
       <c r="C1009" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1010">
@@ -13501,7 +13501,7 @@
         </is>
       </c>
       <c r="C1010" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="1011">
@@ -13514,7 +13514,7 @@
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="1012">
@@ -13553,7 +13553,7 @@
         </is>
       </c>
       <c r="C1014" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1015">
@@ -13566,7 +13566,7 @@
         </is>
       </c>
       <c r="C1015" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1016">
@@ -13579,7 +13579,59 @@
         </is>
       </c>
       <c r="C1016" t="n">
-        <v>15</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="2" t="n">
+        <v>44166</v>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="C1017" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="2" t="n">
+        <v>44166</v>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="C1018" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="2" t="n">
+        <v>44166</v>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="C1019" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="2" t="n">
+        <v>44166</v>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>80+</t>
+        </is>
+      </c>
+      <c r="C1020" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>